<commit_message>
remove trailing white space on label
</commit_message>
<xml_diff>
--- a/data/external/ethikchat_data-main/mensateria_survey/processed/curated/mensateria_survey_autoai_curated_dialogues.xlsx
+++ b/data/external/ethikchat_data-main/mensateria_survey/processed/curated/mensateria_survey_autoai_curated_dialogues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8347" uniqueCount="1852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8347" uniqueCount="1851">
   <si>
     <t xml:space="preserve">Unnamed: 0</t>
   </si>
@@ -5308,9 +5308,6 @@
   </si>
   <si>
     <t xml:space="preserve">Es wäre aber eine doppelte Sicherheit, da zum einen der Mensch eingreifen kann und zum anderen das Auto sehr viel selbst macht </t>
-  </si>
-  <si>
-    <t xml:space="preserve">['Z.C5-1-1-1 ']</t>
   </si>
   <si>
     <t xml:space="preserve">Was sagst du denn zu dem Thema? </t>
@@ -5716,11 +5713,11 @@
   </sheetPr>
   <dimension ref="A1:G1669"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1027" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1053" activeCellId="0" sqref="I1053"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1571" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1590" activeCellId="0" sqref="F1590"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="57.97"/>
@@ -42290,7 +42287,7 @@
         <v>1757</v>
       </c>
       <c r="F1590" s="2" t="s">
-        <v>1758</v>
+        <v>474</v>
       </c>
       <c r="G1590" s="2" t="s">
         <v>1287</v>
@@ -42333,7 +42330,7 @@
         <v>8</v>
       </c>
       <c r="E1592" s="2" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1592" s="2" t="s">
         <v>1702</v>
@@ -42379,7 +42376,7 @@
         <v>8</v>
       </c>
       <c r="E1594" s="2" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1594" s="2" t="s">
         <v>10</v>
@@ -42425,7 +42422,7 @@
         <v>8</v>
       </c>
       <c r="E1596" s="2" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="F1596" s="2" t="s">
         <v>108</v>
@@ -42471,7 +42468,7 @@
         <v>8</v>
       </c>
       <c r="E1598" s="2" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="F1598" s="2" t="s">
         <v>108</v>
@@ -42517,7 +42514,7 @@
         <v>8</v>
       </c>
       <c r="E1600" s="2" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="F1600" s="2" t="s">
         <v>44</v>
@@ -42563,7 +42560,7 @@
         <v>8</v>
       </c>
       <c r="E1602" s="2" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="F1602" s="2" t="s">
         <v>10</v>
@@ -42609,7 +42606,7 @@
         <v>8</v>
       </c>
       <c r="E1604" s="2" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="F1604" s="2" t="s">
         <v>10</v>
@@ -42646,7 +42643,7 @@
         <v>1604</v>
       </c>
       <c r="B1606" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1606" s="2" t="n">
         <v>0</v>
@@ -42655,7 +42652,7 @@
         <v>8</v>
       </c>
       <c r="E1606" s="2" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="F1606" s="2" t="s">
         <v>354</v>
@@ -42669,7 +42666,7 @@
         <v>1605</v>
       </c>
       <c r="B1607" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1607" s="2" t="n">
         <v>1</v>
@@ -42678,13 +42675,13 @@
         <v>12</v>
       </c>
       <c r="E1607" s="2" t="s">
+        <v>1767</v>
+      </c>
+      <c r="F1607" s="2" t="s">
         <v>1768</v>
       </c>
-      <c r="F1607" s="2" t="s">
+      <c r="G1607" s="2" t="s">
         <v>1769</v>
-      </c>
-      <c r="G1607" s="2" t="s">
-        <v>1770</v>
       </c>
     </row>
     <row r="1608" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42692,7 +42689,7 @@
         <v>1606</v>
       </c>
       <c r="B1608" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1608" s="2" t="n">
         <v>2</v>
@@ -42701,7 +42698,7 @@
         <v>8</v>
       </c>
       <c r="E1608" s="2" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="F1608" s="2" t="s">
         <v>102</v>
@@ -42715,7 +42712,7 @@
         <v>1607</v>
       </c>
       <c r="B1609" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1609" s="2" t="n">
         <v>3</v>
@@ -42738,7 +42735,7 @@
         <v>1608</v>
       </c>
       <c r="B1610" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1610" s="2" t="n">
         <v>4</v>
@@ -42747,7 +42744,7 @@
         <v>8</v>
       </c>
       <c r="E1610" s="2" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="F1610" s="2" t="s">
         <v>47</v>
@@ -42761,7 +42758,7 @@
         <v>1609</v>
       </c>
       <c r="B1611" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1611" s="2" t="n">
         <v>5</v>
@@ -42784,7 +42781,7 @@
         <v>1610</v>
       </c>
       <c r="B1612" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1612" s="2" t="n">
         <v>6</v>
@@ -42793,13 +42790,13 @@
         <v>8</v>
       </c>
       <c r="E1612" s="2" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="F1612" s="2" t="s">
         <v>655</v>
       </c>
       <c r="G1612" s="2" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="1613" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42807,7 +42804,7 @@
         <v>1611</v>
       </c>
       <c r="B1613" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1613" s="2" t="n">
         <v>7</v>
@@ -42830,7 +42827,7 @@
         <v>1612</v>
       </c>
       <c r="B1614" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1614" s="2" t="n">
         <v>8</v>
@@ -42839,7 +42836,7 @@
         <v>8</v>
       </c>
       <c r="E1614" s="2" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="F1614" s="2" t="s">
         <v>44</v>
@@ -42853,7 +42850,7 @@
         <v>1613</v>
       </c>
       <c r="B1615" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1615" s="2" t="n">
         <v>9</v>
@@ -42862,13 +42859,13 @@
         <v>12</v>
       </c>
       <c r="E1615" s="2" t="s">
+        <v>1775</v>
+      </c>
+      <c r="F1615" s="2" t="s">
         <v>1776</v>
       </c>
-      <c r="F1615" s="2" t="s">
+      <c r="G1615" s="2" t="s">
         <v>1777</v>
-      </c>
-      <c r="G1615" s="2" t="s">
-        <v>1778</v>
       </c>
     </row>
     <row r="1616" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42876,7 +42873,7 @@
         <v>1614</v>
       </c>
       <c r="B1616" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1616" s="2" t="n">
         <v>10</v>
@@ -42885,7 +42882,7 @@
         <v>8</v>
       </c>
       <c r="E1616" s="2" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="F1616" s="2" t="s">
         <v>112</v>
@@ -42899,7 +42896,7 @@
         <v>1615</v>
       </c>
       <c r="B1617" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1617" s="2" t="n">
         <v>11</v>
@@ -42922,7 +42919,7 @@
         <v>1616</v>
       </c>
       <c r="B1618" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1618" s="2" t="n">
         <v>12</v>
@@ -42931,7 +42928,7 @@
         <v>8</v>
       </c>
       <c r="E1618" s="2" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="F1618" s="2" t="s">
         <v>202</v>
@@ -42945,7 +42942,7 @@
         <v>1617</v>
       </c>
       <c r="B1619" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1619" s="2" t="n">
         <v>13</v>
@@ -42968,7 +42965,7 @@
         <v>1618</v>
       </c>
       <c r="B1620" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1620" s="2" t="n">
         <v>14</v>
@@ -42977,13 +42974,13 @@
         <v>8</v>
       </c>
       <c r="E1620" s="2" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="F1620" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G1620" s="2" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="1621" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42991,7 +42988,7 @@
         <v>1619</v>
       </c>
       <c r="B1621" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1621" s="2" t="n">
         <v>15</v>
@@ -43000,13 +42997,13 @@
         <v>12</v>
       </c>
       <c r="E1621" s="2" t="s">
+        <v>1782</v>
+      </c>
+      <c r="F1621" s="2" t="s">
         <v>1783</v>
       </c>
-      <c r="F1621" s="2" t="s">
+      <c r="G1621" s="2" t="s">
         <v>1784</v>
-      </c>
-      <c r="G1621" s="2" t="s">
-        <v>1785</v>
       </c>
     </row>
     <row r="1622" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43014,7 +43011,7 @@
         <v>1620</v>
       </c>
       <c r="B1622" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1622" s="2" t="n">
         <v>16</v>
@@ -43023,13 +43020,13 @@
         <v>8</v>
       </c>
       <c r="E1622" s="2" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="F1622" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G1622" s="2" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="1623" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43037,7 +43034,7 @@
         <v>1621</v>
       </c>
       <c r="B1623" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1623" s="2" t="n">
         <v>17</v>
@@ -43046,13 +43043,13 @@
         <v>12</v>
       </c>
       <c r="E1623" s="2" t="s">
+        <v>1787</v>
+      </c>
+      <c r="F1623" s="2" t="s">
         <v>1788</v>
       </c>
-      <c r="F1623" s="2" t="s">
+      <c r="G1623" s="2" t="s">
         <v>1789</v>
-      </c>
-      <c r="G1623" s="2" t="s">
-        <v>1790</v>
       </c>
     </row>
     <row r="1624" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43060,7 +43057,7 @@
         <v>1622</v>
       </c>
       <c r="B1624" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1624" s="2" t="n">
         <v>18</v>
@@ -43069,13 +43066,13 @@
         <v>8</v>
       </c>
       <c r="E1624" s="2" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="F1624" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G1624" s="2" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="1625" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43083,7 +43080,7 @@
         <v>1623</v>
       </c>
       <c r="B1625" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1625" s="2" t="n">
         <v>19</v>
@@ -43092,13 +43089,13 @@
         <v>12</v>
       </c>
       <c r="E1625" s="2" t="s">
+        <v>1792</v>
+      </c>
+      <c r="F1625" s="2" t="s">
         <v>1793</v>
       </c>
-      <c r="F1625" s="2" t="s">
+      <c r="G1625" s="2" t="s">
         <v>1794</v>
-      </c>
-      <c r="G1625" s="2" t="s">
-        <v>1795</v>
       </c>
     </row>
     <row r="1626" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43106,7 +43103,7 @@
         <v>1624</v>
       </c>
       <c r="B1626" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1626" s="2" t="n">
         <v>20</v>
@@ -43115,13 +43112,13 @@
         <v>8</v>
       </c>
       <c r="E1626" s="2" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="F1626" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G1626" s="2" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="1627" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43129,7 +43126,7 @@
         <v>1625</v>
       </c>
       <c r="B1627" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1627" s="2" t="n">
         <v>21</v>
@@ -43138,13 +43135,13 @@
         <v>12</v>
       </c>
       <c r="E1627" s="2" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F1627" s="2" t="s">
         <v>1798</v>
       </c>
-      <c r="F1627" s="2" t="s">
+      <c r="G1627" s="2" t="s">
         <v>1799</v>
-      </c>
-      <c r="G1627" s="2" t="s">
-        <v>1800</v>
       </c>
     </row>
     <row r="1628" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43152,7 +43149,7 @@
         <v>1626</v>
       </c>
       <c r="B1628" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1628" s="2" t="n">
         <v>22</v>
@@ -43161,13 +43158,13 @@
         <v>8</v>
       </c>
       <c r="E1628" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="F1628" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G1628" s="2" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="1629" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43175,7 +43172,7 @@
         <v>1627</v>
       </c>
       <c r="B1629" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1629" s="2" t="n">
         <v>23</v>
@@ -43184,13 +43181,13 @@
         <v>12</v>
       </c>
       <c r="E1629" s="2" t="s">
+        <v>1802</v>
+      </c>
+      <c r="F1629" s="2" t="s">
         <v>1803</v>
       </c>
-      <c r="F1629" s="2" t="s">
+      <c r="G1629" s="2" t="s">
         <v>1804</v>
-      </c>
-      <c r="G1629" s="2" t="s">
-        <v>1805</v>
       </c>
     </row>
     <row r="1630" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43198,7 +43195,7 @@
         <v>1628</v>
       </c>
       <c r="B1630" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1630" s="2" t="n">
         <v>24</v>
@@ -43207,13 +43204,13 @@
         <v>8</v>
       </c>
       <c r="E1630" s="2" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="F1630" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G1630" s="2" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="1631" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43221,7 +43218,7 @@
         <v>1629</v>
       </c>
       <c r="B1631" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1631" s="2" t="n">
         <v>25</v>
@@ -43230,13 +43227,13 @@
         <v>12</v>
       </c>
       <c r="E1631" s="2" t="s">
+        <v>1807</v>
+      </c>
+      <c r="F1631" s="2" t="s">
         <v>1808</v>
       </c>
-      <c r="F1631" s="2" t="s">
+      <c r="G1631" s="2" t="s">
         <v>1809</v>
-      </c>
-      <c r="G1631" s="2" t="s">
-        <v>1810</v>
       </c>
     </row>
     <row r="1632" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43244,7 +43241,7 @@
         <v>1630</v>
       </c>
       <c r="B1632" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1632" s="2" t="n">
         <v>26</v>
@@ -43253,13 +43250,13 @@
         <v>8</v>
       </c>
       <c r="E1632" s="2" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="F1632" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G1632" s="2" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="1633" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43267,7 +43264,7 @@
         <v>1631</v>
       </c>
       <c r="B1633" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1633" s="2" t="n">
         <v>27</v>
@@ -43276,13 +43273,13 @@
         <v>12</v>
       </c>
       <c r="E1633" s="2" t="s">
+        <v>1812</v>
+      </c>
+      <c r="F1633" s="2" t="s">
         <v>1813</v>
       </c>
-      <c r="F1633" s="2" t="s">
+      <c r="G1633" s="2" t="s">
         <v>1814</v>
-      </c>
-      <c r="G1633" s="2" t="s">
-        <v>1815</v>
       </c>
     </row>
     <row r="1634" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43290,7 +43287,7 @@
         <v>1632</v>
       </c>
       <c r="B1634" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1634" s="2" t="n">
         <v>28</v>
@@ -43299,7 +43296,7 @@
         <v>8</v>
       </c>
       <c r="E1634" s="2" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="F1634" s="2" t="s">
         <v>102</v>
@@ -43313,7 +43310,7 @@
         <v>1633</v>
       </c>
       <c r="B1635" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1635" s="2" t="n">
         <v>29</v>
@@ -43336,7 +43333,7 @@
         <v>1634</v>
       </c>
       <c r="B1636" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1636" s="2" t="n">
         <v>30</v>
@@ -43345,7 +43342,7 @@
         <v>8</v>
       </c>
       <c r="E1636" s="2" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="F1636" s="2" t="s">
         <v>102</v>
@@ -43359,7 +43356,7 @@
         <v>1635</v>
       </c>
       <c r="B1637" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1637" s="2" t="n">
         <v>31</v>
@@ -43368,13 +43365,13 @@
         <v>12</v>
       </c>
       <c r="E1637" s="2" t="s">
+        <v>1817</v>
+      </c>
+      <c r="F1637" s="2" t="s">
         <v>1818</v>
       </c>
-      <c r="F1637" s="2" t="s">
+      <c r="G1637" s="2" t="s">
         <v>1819</v>
-      </c>
-      <c r="G1637" s="2" t="s">
-        <v>1820</v>
       </c>
     </row>
     <row r="1638" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43382,7 +43379,7 @@
         <v>1636</v>
       </c>
       <c r="B1638" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1638" s="2" t="n">
         <v>32</v>
@@ -43391,13 +43388,13 @@
         <v>8</v>
       </c>
       <c r="E1638" s="2" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="F1638" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G1638" s="2" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="1639" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43405,7 +43402,7 @@
         <v>1637</v>
       </c>
       <c r="B1639" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1639" s="2" t="n">
         <v>33</v>
@@ -43428,7 +43425,7 @@
         <v>1638</v>
       </c>
       <c r="B1640" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1640" s="2" t="n">
         <v>34</v>
@@ -43437,7 +43434,7 @@
         <v>8</v>
       </c>
       <c r="E1640" s="2" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="F1640" s="2" t="s">
         <v>202</v>
@@ -43451,7 +43448,7 @@
         <v>1639</v>
       </c>
       <c r="B1641" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1641" s="2" t="n">
         <v>35</v>
@@ -43460,13 +43457,13 @@
         <v>12</v>
       </c>
       <c r="E1641" s="2" t="s">
+        <v>1823</v>
+      </c>
+      <c r="F1641" s="2" t="s">
         <v>1824</v>
       </c>
-      <c r="F1641" s="2" t="s">
+      <c r="G1641" s="2" t="s">
         <v>1825</v>
-      </c>
-      <c r="G1641" s="2" t="s">
-        <v>1826</v>
       </c>
     </row>
     <row r="1642" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43474,7 +43471,7 @@
         <v>1640</v>
       </c>
       <c r="B1642" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1642" s="2" t="n">
         <v>36</v>
@@ -43483,13 +43480,13 @@
         <v>8</v>
       </c>
       <c r="E1642" s="2" t="s">
+        <v>1826</v>
+      </c>
+      <c r="F1642" s="2" t="s">
         <v>1827</v>
       </c>
-      <c r="F1642" s="2" t="s">
+      <c r="G1642" s="2" t="s">
         <v>1828</v>
-      </c>
-      <c r="G1642" s="2" t="s">
-        <v>1829</v>
       </c>
     </row>
     <row r="1643" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43497,7 +43494,7 @@
         <v>1641</v>
       </c>
       <c r="B1643" s="2" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="C1643" s="2" t="n">
         <v>37</v>
@@ -43520,7 +43517,7 @@
         <v>1642</v>
       </c>
       <c r="B1644" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1644" s="2" t="n">
         <v>0</v>
@@ -43529,7 +43526,7 @@
         <v>8</v>
       </c>
       <c r="E1644" s="2" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="F1644" s="2" t="s">
         <v>1669</v>
@@ -43543,7 +43540,7 @@
         <v>1643</v>
       </c>
       <c r="B1645" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1645" s="2" t="n">
         <v>1</v>
@@ -43566,7 +43563,7 @@
         <v>1644</v>
       </c>
       <c r="B1646" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1646" s="2" t="n">
         <v>2</v>
@@ -43575,7 +43572,7 @@
         <v>8</v>
       </c>
       <c r="E1646" s="2" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="F1646" s="2" t="s">
         <v>1669</v>
@@ -43589,7 +43586,7 @@
         <v>1645</v>
       </c>
       <c r="B1647" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1647" s="2" t="n">
         <v>3</v>
@@ -43598,13 +43595,13 @@
         <v>12</v>
       </c>
       <c r="E1647" s="2" t="s">
+        <v>1832</v>
+      </c>
+      <c r="F1647" s="2" t="s">
         <v>1833</v>
       </c>
-      <c r="F1647" s="2" t="s">
+      <c r="G1647" s="2" t="s">
         <v>1834</v>
-      </c>
-      <c r="G1647" s="2" t="s">
-        <v>1835</v>
       </c>
     </row>
     <row r="1648" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43612,7 +43609,7 @@
         <v>1646</v>
       </c>
       <c r="B1648" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1648" s="2" t="n">
         <v>4</v>
@@ -43621,7 +43618,7 @@
         <v>8</v>
       </c>
       <c r="E1648" s="2" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="F1648" s="2" t="s">
         <v>655</v>
@@ -43635,7 +43632,7 @@
         <v>1647</v>
       </c>
       <c r="B1649" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1649" s="2" t="n">
         <v>5</v>
@@ -43658,7 +43655,7 @@
         <v>1648</v>
       </c>
       <c r="B1650" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1650" s="2" t="n">
         <v>6</v>
@@ -43667,7 +43664,7 @@
         <v>8</v>
       </c>
       <c r="E1650" s="2" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="F1650" s="2" t="s">
         <v>655</v>
@@ -43681,7 +43678,7 @@
         <v>1649</v>
       </c>
       <c r="B1651" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1651" s="2" t="n">
         <v>7</v>
@@ -43704,7 +43701,7 @@
         <v>1650</v>
       </c>
       <c r="B1652" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1652" s="2" t="n">
         <v>8</v>
@@ -43713,7 +43710,7 @@
         <v>8</v>
       </c>
       <c r="E1652" s="2" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="F1652" s="2" t="s">
         <v>354</v>
@@ -43727,7 +43724,7 @@
         <v>1651</v>
       </c>
       <c r="B1653" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1653" s="2" t="n">
         <v>9</v>
@@ -43750,7 +43747,7 @@
         <v>1652</v>
       </c>
       <c r="B1654" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1654" s="2" t="n">
         <v>10</v>
@@ -43759,7 +43756,7 @@
         <v>8</v>
       </c>
       <c r="E1654" s="2" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="F1654" s="2" t="s">
         <v>354</v>
@@ -43773,7 +43770,7 @@
         <v>1653</v>
       </c>
       <c r="B1655" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1655" s="2" t="n">
         <v>11</v>
@@ -43782,13 +43779,13 @@
         <v>12</v>
       </c>
       <c r="E1655" s="2" t="s">
+        <v>1838</v>
+      </c>
+      <c r="F1655" s="2" t="s">
         <v>1839</v>
       </c>
-      <c r="F1655" s="2" t="s">
+      <c r="G1655" s="2" t="s">
         <v>1840</v>
-      </c>
-      <c r="G1655" s="2" t="s">
-        <v>1841</v>
       </c>
     </row>
     <row r="1656" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43796,7 +43793,7 @@
         <v>1654</v>
       </c>
       <c r="B1656" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1656" s="2" t="n">
         <v>12</v>
@@ -43819,7 +43816,7 @@
         <v>1655</v>
       </c>
       <c r="B1657" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1657" s="2" t="n">
         <v>13</v>
@@ -43842,7 +43839,7 @@
         <v>1656</v>
       </c>
       <c r="B1658" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1658" s="2" t="n">
         <v>14</v>
@@ -43851,7 +43848,7 @@
         <v>8</v>
       </c>
       <c r="E1658" s="2" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="F1658" s="2" t="s">
         <v>937</v>
@@ -43865,7 +43862,7 @@
         <v>1657</v>
       </c>
       <c r="B1659" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1659" s="2" t="n">
         <v>15</v>
@@ -43888,7 +43885,7 @@
         <v>1658</v>
       </c>
       <c r="B1660" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1660" s="2" t="n">
         <v>16</v>
@@ -43897,7 +43894,7 @@
         <v>8</v>
       </c>
       <c r="E1660" s="2" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="F1660" s="2" t="s">
         <v>102</v>
@@ -43911,7 +43908,7 @@
         <v>1659</v>
       </c>
       <c r="B1661" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1661" s="2" t="n">
         <v>17</v>
@@ -43934,7 +43931,7 @@
         <v>1660</v>
       </c>
       <c r="B1662" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1662" s="2" t="n">
         <v>18</v>
@@ -43943,7 +43940,7 @@
         <v>8</v>
       </c>
       <c r="E1662" s="2" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="F1662" s="2" t="s">
         <v>102</v>
@@ -43957,7 +43954,7 @@
         <v>1661</v>
       </c>
       <c r="B1663" s="2" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="C1663" s="2" t="n">
         <v>19</v>
@@ -43966,13 +43963,13 @@
         <v>12</v>
       </c>
       <c r="E1663" s="2" t="s">
+        <v>1844</v>
+      </c>
+      <c r="F1663" s="2" t="s">
         <v>1845</v>
       </c>
-      <c r="F1663" s="2" t="s">
+      <c r="G1663" s="2" t="s">
         <v>1846</v>
-      </c>
-      <c r="G1663" s="2" t="s">
-        <v>1847</v>
       </c>
     </row>
     <row r="1664" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43980,7 +43977,7 @@
         <v>1662</v>
       </c>
       <c r="B1664" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="C1664" s="2" t="n">
         <v>0</v>
@@ -43989,7 +43986,7 @@
         <v>8</v>
       </c>
       <c r="E1664" s="2" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="F1664" s="2" t="s">
         <v>548</v>
@@ -44003,7 +44000,7 @@
         <v>1663</v>
       </c>
       <c r="B1665" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="C1665" s="2" t="n">
         <v>1</v>
@@ -44026,7 +44023,7 @@
         <v>1664</v>
       </c>
       <c r="B1666" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="C1666" s="2" t="n">
         <v>2</v>
@@ -44035,7 +44032,7 @@
         <v>8</v>
       </c>
       <c r="E1666" s="2" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="F1666" s="2" t="s">
         <v>548</v>
@@ -44049,7 +44046,7 @@
         <v>1665</v>
       </c>
       <c r="B1667" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="C1667" s="2" t="n">
         <v>3</v>
@@ -44072,7 +44069,7 @@
         <v>1666</v>
       </c>
       <c r="B1668" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="C1668" s="2" t="n">
         <v>4</v>
@@ -44081,7 +44078,7 @@
         <v>8</v>
       </c>
       <c r="E1668" s="2" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="F1668" s="2" t="s">
         <v>581</v>
@@ -44095,7 +44092,7 @@
         <v>1667</v>
       </c>
       <c r="B1669" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="C1669" s="2" t="n">
         <v>5</v>

</xml_diff>